<commit_message>
encontrando novas redes para o ensemble
</commit_message>
<xml_diff>
--- a/fuction_ensemble_3/fixed_results.xlsx
+++ b/fuction_ensemble_3/fixed_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -971,6 +971,762 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>model_24_9_8</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.9978655741283762</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.9947922486835233</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.9999999999638428</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.9999999999982546</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.9999999999956094</v>
+      </c>
+      <c r="H9" t="n">
+        <v>805.7457665380091</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1965.92612196995</v>
+      </c>
+      <c r="J9" t="n">
+        <v>6.915070117300554e-08</v>
+      </c>
+      <c r="K9" t="n">
+        <v>3.166496753692627e-08</v>
+      </c>
+      <c r="L9" t="n">
+        <v>5.04078343549659e-08</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.01520044360584701</v>
+      </c>
+      <c r="N9" t="n">
+        <v>28.38566128414149</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1.003013307112881</v>
+      </c>
+      <c r="P9" t="n">
+        <v>29.59409765142678</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>68.61646346676432</v>
+      </c>
+      <c r="R9" t="n">
+        <v>118.5903722863605</v>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Hidden Size=[10], regularizer=0.05, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>model_2_8_14</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.999992187636361</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.9929823568752489</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.9999999792930766</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.9999999258332494</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.9999999621547906</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2.949167273715139</v>
+      </c>
+      <c r="I10" t="n">
+        <v>2649.160279593511</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.008462013676762581</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.01518506277352571</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.01182353822514415</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.0006915313058469639</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1.7173139706283</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.999937501090888</v>
+      </c>
+      <c r="P10" t="n">
+        <v>1.790423581687943</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>39.83695429918672</v>
+      </c>
+      <c r="R10" t="n">
+        <v>65.43334662141892</v>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>Hidden Size=[5], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>model_30_8_1</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.9999798916619582</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.9920799592153482</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.9999912860188963</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.9999514375878201</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.9999912991856549</v>
+      </c>
+      <c r="H11" t="n">
+        <v>7.59089761078358</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2989.815396206057</v>
+      </c>
+      <c r="J11" t="n">
+        <v>8.854970594868064</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2.154577646637335</v>
+      </c>
+      <c r="L11" t="n">
+        <v>5.5047741207527</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.007582843109937573</v>
+      </c>
+      <c r="N11" t="n">
+        <v>2.755158364011692</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1.00001930400452</v>
+      </c>
+      <c r="P11" t="n">
+        <v>2.872451159531733</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>93.94610030658913</v>
+      </c>
+      <c r="R11" t="n">
+        <v>153.671015725131</v>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Hidden Size=[12], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>model_8_7_0</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.9997581007167586</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.9942930704440628</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.9991719418988624</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.9999816159005624</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.9999890519567246</v>
+      </c>
+      <c r="H12" t="n">
+        <v>91.31697942361235</v>
+      </c>
+      <c r="I12" t="n">
+        <v>2154.365907366299</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2.722241007490078</v>
+      </c>
+      <c r="K12" t="n">
+        <v>11.45177151635289</v>
+      </c>
+      <c r="L12" t="n">
+        <v>7.087006261921485</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.01626477638597697</v>
+      </c>
+      <c r="N12" t="n">
+        <v>9.555991807427022</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1.005805582797793</v>
+      </c>
+      <c r="P12" t="n">
+        <v>9.962810162299261</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>40.97132651143687</v>
+      </c>
+      <c r="R12" t="n">
+        <v>71.44322213314189</v>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>Hidden Size=[6], regularizer=0.05, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>model_38_7_24</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.9996228785405012</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.9923654502610046</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.999951498895257</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.9999999999971473</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.9999609371212409</v>
+      </c>
+      <c r="H13" t="n">
+        <v>142.3633509607986</v>
+      </c>
+      <c r="I13" t="n">
+        <v>2882.042526470733</v>
+      </c>
+      <c r="J13" t="n">
+        <v>22.25018493272388</v>
+      </c>
+      <c r="K13" t="n">
+        <v>2.952292561531067e-07</v>
+      </c>
+      <c r="L13" t="n">
+        <v>11.12509261164826</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.03608018069230119</v>
+      </c>
+      <c r="N13" t="n">
+        <v>11.93161141509388</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1.000274270152363</v>
+      </c>
+      <c r="P13" t="n">
+        <v>12.43956481487503</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>104.08323480199</v>
+      </c>
+      <c r="R13" t="n">
+        <v>173.5591568194774</v>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>Hidden Size=[14], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>model_26_4_3</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.9994234533115562</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.9924212003350947</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.999913523046573</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.9999999999898611</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.9999201570513343</v>
+      </c>
+      <c r="H14" t="n">
+        <v>217.646374887526</v>
+      </c>
+      <c r="I14" t="n">
+        <v>2860.996873501741</v>
+      </c>
+      <c r="J14" t="n">
+        <v>40.49756265059114</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1.867301762303528e-07</v>
+      </c>
+      <c r="L14" t="n">
+        <v>20.24916981847491</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.04177834619065011</v>
+      </c>
+      <c r="N14" t="n">
+        <v>14.75284294254928</v>
+      </c>
+      <c r="O14" t="n">
+        <v>1.000658910501079</v>
+      </c>
+      <c r="P14" t="n">
+        <v>15.38090200920857</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>79.23425677567501</v>
+      </c>
+      <c r="R14" t="n">
+        <v>134.083668894744</v>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>Hidden Size=[11], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>model_35_7_20</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.9976680892119211</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9907276899732727</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.9998407683893979</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.9999065008447229</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.9998789068593676</v>
+      </c>
+      <c r="H15" t="n">
+        <v>880.2963224998115</v>
+      </c>
+      <c r="I15" t="n">
+        <v>3500.297035089578</v>
+      </c>
+      <c r="J15" t="n">
+        <v>58.06455320422538</v>
+      </c>
+      <c r="K15" t="n">
+        <v>36.84860146441497</v>
+      </c>
+      <c r="L15" t="n">
+        <v>47.45597609574907</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.1152202243137621</v>
+      </c>
+      <c r="N15" t="n">
+        <v>29.66978804271799</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1.001929857203927</v>
+      </c>
+      <c r="P15" t="n">
+        <v>30.93289234462473</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>92.43948283819037</v>
+      </c>
+      <c r="R15" t="n">
+        <v>157.039901556205</v>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>Hidden Size=[13], regularizer=0.05, learning_rate=0.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>model_18_8_24</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.9999120808381883</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.993368293836536</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.9998087303952133</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.9998677464268457</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.9998557449108948</v>
+      </c>
+      <c r="H16" t="n">
+        <v>33.18948358390484</v>
+      </c>
+      <c r="I16" t="n">
+        <v>2503.46907670764</v>
+      </c>
+      <c r="J16" t="n">
+        <v>56.39823384140618</v>
+      </c>
+      <c r="K16" t="n">
+        <v>150.1367359992585</v>
+      </c>
+      <c r="L16" t="n">
+        <v>103.2674849203323</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.01379699485226435</v>
+      </c>
+      <c r="N16" t="n">
+        <v>5.761031468748008</v>
+      </c>
+      <c r="O16" t="n">
+        <v>1.000162312298729</v>
+      </c>
+      <c r="P16" t="n">
+        <v>6.006290505351799</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>66.99553386755478</v>
+      </c>
+      <c r="R16" t="n">
+        <v>112.0939393876782</v>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>Hidden Size=[9], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>model_118_8_22</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0.9999976329375331</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.9930579544873804</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.9999987961061981</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.9999999910900658</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.9999999535882388</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.8935660812631268</v>
+      </c>
+      <c r="I17" t="n">
+        <v>2620.622181013896</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.05142131401225924</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.006023936904966831</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.02872262545861304</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.002968030022015975</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.9452862430307165</v>
+      </c>
+      <c r="O17" t="n">
+        <v>1.000056809499206</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.9855290354088171</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>50.22506997870457</v>
+      </c>
+      <c r="R17" t="n">
+        <v>80.69696560040958</v>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>Hidden Size=[3, 3], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>model_21_9_0</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.9999197326609552</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.992652573302916</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.9998916382681973</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.9999221223374015</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.9999164517386357</v>
+      </c>
+      <c r="H18" t="n">
+        <v>30.30092048939316</v>
+      </c>
+      <c r="I18" t="n">
+        <v>2773.653578149225</v>
+      </c>
+      <c r="J18" t="n">
+        <v>98.80879856832325</v>
+      </c>
+      <c r="K18" t="n">
+        <v>9.176300647202879</v>
+      </c>
+      <c r="L18" t="n">
+        <v>53.99241118587088</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.03222094239256876</v>
+      </c>
+      <c r="N18" t="n">
+        <v>5.504627188955957</v>
+      </c>
+      <c r="O18" t="n">
+        <v>1.000275202305296</v>
+      </c>
+      <c r="P18" t="n">
+        <v>5.73897056453897</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>55.17764381751644</v>
+      </c>
+      <c r="R18" t="n">
+        <v>92.96279438843065</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>Hidden Size=[4, 3], regularizer=0.2, learning_rate=0.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>model_7_9_0</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.9998326480363232</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.9923832218103555</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.9999225595991194</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.9998541490986304</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.9998911204576901</v>
+      </c>
+      <c r="H19" t="n">
+        <v>63.1753662879765</v>
+      </c>
+      <c r="I19" t="n">
+        <v>2875.333766590793</v>
+      </c>
+      <c r="J19" t="n">
+        <v>13.79733842378482</v>
+      </c>
+      <c r="K19" t="n">
+        <v>39.84897306654602</v>
+      </c>
+      <c r="L19" t="n">
+        <v>26.82315574516542</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.04225721428789764</v>
+      </c>
+      <c r="N19" t="n">
+        <v>7.948293294033411</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.9991967105743514</v>
+      </c>
+      <c r="P19" t="n">
+        <v>8.286668594795767</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>29.70817109750642</v>
+      </c>
+      <c r="R19" t="n">
+        <v>52.86681177000224</v>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Hidden Size=[2, 3], regularizer=0.05, learning_rate=0.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>model_29_6_0</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9994984885356603</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.9938387948817379</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.9999486632114739</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.9998119424085081</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.9998516841850127</v>
+      </c>
+      <c r="H20" t="n">
+        <v>189.3205777882411</v>
+      </c>
+      <c r="I20" t="n">
+        <v>2325.85493214396</v>
+      </c>
+      <c r="J20" t="n">
+        <v>5.169935459503904</v>
+      </c>
+      <c r="K20" t="n">
+        <v>66.00821461365558</v>
+      </c>
+      <c r="L20" t="n">
+        <v>35.58907503657974</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.08809317910641791</v>
+      </c>
+      <c r="N20" t="n">
+        <v>13.7593814464256</v>
+      </c>
+      <c r="O20" t="n">
+        <v>1.000633488165482</v>
+      </c>
+      <c r="P20" t="n">
+        <v>14.3451468004461</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>75.51311648610645</v>
+      </c>
+      <c r="R20" t="n">
+        <v>127.9247769554391</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Hidden Size=[2, 9], regularizer=0.2, learning_rate=0.01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>